<commit_message>
hooked up public Google Sheets to Open Procure application
</commit_message>
<xml_diff>
--- a/google_drive_cache/13nyHeQDzZ2zRgDu87MmZiRoF6Uk_tXGBOpYLD07Aj94.xlsx
+++ b/google_drive_cache/13nyHeQDzZ2zRgDu87MmZiRoF6Uk_tXGBOpYLD07Aj94.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="procurement" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -489,7 +489,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="2">
-        <v>100000.0</v>
+        <v>20000.0</v>
       </c>
       <c r="E2" s="1">
         <v>1418788.0</v>

</xml_diff>